<commit_message>
added create_data_from_from_log to follow_up_queries. Not sure if this is the best way to do this
</commit_message>
<xml_diff>
--- a/logs/Follow_Up_Log.xlsx
+++ b/logs/Follow_Up_Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="562">
   <si>
     <t xml:space="preserve">SubjectID</t>
   </si>
@@ -1714,8 +1714,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1782,12 +1783,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1811,19 +1816,19 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2020,8 +2025,8 @@
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
+      <c r="D9" s="2" t="n">
+        <v>43040</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>33</v>
@@ -2043,8 +2048,8 @@
       <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
+      <c r="D10" s="2" t="n">
+        <v>43041</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>36</v>
@@ -2066,8 +2071,8 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
+      <c r="D11" s="2" t="n">
+        <v>43042</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>39</v>
@@ -2089,8 +2094,8 @@
       <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
+      <c r="D12" s="2" t="n">
+        <v>43043</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>42</v>
@@ -2112,8 +2117,8 @@
       <c r="C13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
+      <c r="D13" s="2" t="n">
+        <v>43044</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>45</v>
@@ -6468,12 +6473,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6494,12 +6499,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed data_request_functions, had incorrect day, month, year order and hour, minute order. Time to research pytest and make some test to confirm my inputs are getting the right types of inputs.
Added get_follow_up_by_custom_date to follow_up_queries
</commit_message>
<xml_diff>
--- a/logs/Follow_Up_Log.xlsx
+++ b/logs/Follow_Up_Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="562">
   <si>
     <t xml:space="preserve">SubjectID</t>
   </si>
@@ -1816,19 +1816,19 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.0102040816327"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2002,8 +2002,8 @@
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
+      <c r="D8" s="2" t="n">
+        <v>43042</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>30</v>
@@ -6478,7 +6478,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6504,7 +6504,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>